<commit_message>
program output new data and duplicate code
</commit_message>
<xml_diff>
--- a/ArrayFromPycharm.xlsx
+++ b/ArrayFromPycharm.xlsx
@@ -366,13 +366,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:3">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -382,28 +382,10 @@
       <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:3">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -411,255 +393,27 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>